<commit_message>
Updated components and their xlsx files
</commit_message>
<xml_diff>
--- a/batterypacks.xlsx
+++ b/batterypacks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t/>
   </si>
@@ -19,9 +19,18 @@
     <t>ADV</t>
   </si>
   <si>
+    <t>ADV 2</t>
+  </si>
+  <si>
     <t>ADV Pro</t>
   </si>
   <si>
+    <t>CBGT 50S</t>
+  </si>
+  <si>
+    <t>CBGT P42A</t>
+  </si>
+  <si>
     <t>CBSP</t>
   </si>
   <si>
@@ -64,7 +73,10 @@
     <t>Pint X</t>
   </si>
   <si>
-    <t>SUPzero</t>
+    <t>Quart</t>
+  </si>
+  <si>
+    <t>Quart S Edition</t>
   </si>
   <si>
     <t>XR</t>
@@ -79,9 +91,18 @@
     <t>Floatwheel ADV battery pack. This pack was originally said to be built with DG40 batteries, but I'm not sure if those even exist. They are now advertised to contain LR2170LA batteries</t>
   </si>
   <si>
+    <t>Floatwheel ADV 2 battery pack.</t>
+  </si>
+  <si>
     <t>Floatwheel ADV Pro battery pack.</t>
   </si>
   <si>
+    <t>Onewheel GT upgrade 50S edition</t>
+  </si>
+  <si>
+    <t>Onewheel GT upgrade</t>
+  </si>
+  <si>
     <t>Chi Batteries - XR Stunt Pack.</t>
   </si>
   <si>
@@ -106,7 +127,10 @@
     <t>Original Pint X battery pack.</t>
   </si>
   <si>
-    <t>SUPzero's own favorite. Much torque, not too much speed, not too heavy. Not commercially available. I added it here because it is my own favorite pack, and this is my web tool, so why not :)</t>
+    <t>Onewheel Pint upgrade</t>
+  </si>
+  <si>
+    <t>Onewheel Pint upgrade with 50S batteries</t>
   </si>
   <si>
     <t>Original Onewheel XR battery pack.</t>
@@ -124,13 +148,16 @@
     <t>LR2170LA</t>
   </si>
   <si>
+    <t>50S</t>
+  </si>
+  <si>
     <t>P42A</t>
   </si>
   <si>
     <t>M35A</t>
   </si>
   <si>
-    <t>50S</t>
+    <t>P45B</t>
   </si>
   <si>
     <t>VTC6</t>
@@ -154,6 +181,9 @@
     <t>https://floatwheels.ru/index.php?route=product/product&amp;product_id=9904</t>
   </si>
   <si>
+    <t>https://chibatterysystems.com/collections/onewheel/products/cbgt</t>
+  </si>
+  <si>
     <t>https://chibatterysystems.com/collections/onewheel-xr/products/cbsp</t>
   </si>
   <si>
@@ -172,7 +202,10 @@
     <t>https://theboardgarage.com/articles/pint-x-battery-repair-balance-wires-amp-broken-solder-joint</t>
   </si>
   <si>
-    <t>https://supzero.ch/making-a-21700-16s2p-battery-pack/</t>
+    <t>https://chibatterysystems.com/collections/onewheel/products/quart?variant=44340683866357</t>
+  </si>
+  <si>
+    <t>https://chibatterysystems.com/collections/onewheel/products/quart?variant=44340683899125</t>
   </si>
   <si>
     <t>https://web.archive.org/web/20211028001953/https://onewheel.com/products/xr</t>
@@ -574,7 +607,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -583,10 +616,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="19" width="15.037593984962404" customWidth="1"/>
+    <col min="1" max="23" width="12.422360248447205" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -644,10 +677,22 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -703,143 +748,195 @@
       <c r="S2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="T2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="G4" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
-      <c r="S4" s="3" t="s">
-        <v>34</v>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>41</v>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3">
         <v>20</v>
@@ -848,57 +945,69 @@
         <v>20</v>
       </c>
       <c r="D6" s="3">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3">
+        <v>15</v>
+      </c>
+      <c r="H6" s="3">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3">
+        <v>18</v>
+      </c>
+      <c r="K6" s="3">
+        <v>27</v>
+      </c>
+      <c r="L6" s="3">
+        <v>15</v>
+      </c>
+      <c r="M6" s="3">
+        <v>16</v>
+      </c>
+      <c r="N6" s="3">
+        <v>18</v>
+      </c>
+      <c r="O6" s="3">
         <v>19</v>
       </c>
-      <c r="E6" s="3">
+      <c r="P6" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>24</v>
+      </c>
+      <c r="R6" s="3">
+        <v>27</v>
+      </c>
+      <c r="S6" s="3">
+        <v>30</v>
+      </c>
+      <c r="T6" s="3">
         <v>15</v>
       </c>
-      <c r="F6" s="3">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3">
-        <v>18</v>
-      </c>
-      <c r="H6" s="3">
-        <v>27</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="U6" s="3">
         <v>15</v>
       </c>
-      <c r="J6" s="3">
-        <v>16</v>
-      </c>
-      <c r="K6" s="3">
-        <v>18</v>
-      </c>
-      <c r="L6" s="3">
-        <v>19</v>
-      </c>
-      <c r="M6" s="3">
-        <v>20</v>
-      </c>
-      <c r="N6" s="3">
-        <v>24</v>
-      </c>
-      <c r="O6" s="3">
-        <v>27</v>
-      </c>
-      <c r="P6" s="3">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="3">
+      <c r="V6" s="3">
         <v>15</v>
       </c>
-      <c r="R6" s="3">
-        <v>16</v>
-      </c>
-      <c r="S6" s="3">
+      <c r="W6" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -907,29 +1016,29 @@
         <v>2</v>
       </c>
       <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="3">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2</v>
-      </c>
       <c r="H7" s="3">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
         <v>1</v>
       </c>
-      <c r="I7" s="3">
-        <v>2</v>
-      </c>
-      <c r="J7" s="3">
-        <v>2</v>
-      </c>
-      <c r="K7" s="3">
-        <v>2</v>
-      </c>
       <c r="L7" s="3">
         <v>2</v>
       </c>
@@ -940,54 +1049,66 @@
         <v>2</v>
       </c>
       <c r="O7" s="3">
+        <v>2</v>
+      </c>
+      <c r="P7" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>2</v>
+      </c>
+      <c r="R7" s="3">
         <v>1</v>
       </c>
-      <c r="P7" s="3">
+      <c r="S7" s="3">
         <v>1</v>
       </c>
-      <c r="Q7" s="3">
-        <v>2</v>
-      </c>
-      <c r="R7" s="3">
-        <v>2</v>
-      </c>
-      <c r="S7" s="3">
+      <c r="T7" s="3">
+        <v>2</v>
+      </c>
+      <c r="U7" s="3">
+        <v>1</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1</v>
+      </c>
+      <c r="W7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>0</v>
@@ -1004,14 +1125,26 @@
       <c r="P8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>54</v>
+      <c r="Q8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1023,9 +1156,13 @@
     <hyperlink ref="F8" r:id="rId5"/>
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="Q8" r:id="rId8"/>
-    <hyperlink ref="R8" r:id="rId9"/>
-    <hyperlink ref="S8" r:id="rId10"/>
+    <hyperlink ref="I8" r:id="rId8"/>
+    <hyperlink ref="J8" r:id="rId9"/>
+    <hyperlink ref="K8" r:id="rId10"/>
+    <hyperlink ref="T8" r:id="rId11"/>
+    <hyperlink ref="U8" r:id="rId12"/>
+    <hyperlink ref="V8" r:id="rId13"/>
+    <hyperlink ref="W8" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>